<commit_message>
update sitemap - assignee列の削除
</commit_message>
<xml_diff>
--- a/px-files/sitemaps/sitemap.xlsx
+++ b/px-files/sitemaps/sitemap.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\pickles2-web\preset-pickles2-webtool-develop\px-files\sitemaps\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32380" yWindow="1440" windowWidth="31260" windowHeight="17640"/>
+    <workbookView xWindow="32385" yWindow="1440" windowWidth="31260" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sitemap" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.7-alpha.1%2Bnb</t>
   </si>
@@ -78,9 +83,6 @@
     <t>削除フラグ</t>
   </si>
   <si>
-    <t>assignee</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -138,9 +140,6 @@
     <t>top</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
     <t>サンプルページ1</t>
   </si>
   <si>
@@ -175,9 +174,6 @@
   </si>
   <si>
     <t>/sample_pages/page5/</t>
-  </si>
-  <si>
-    <t>user2</t>
   </si>
   <si>
     <t>サンプルページ6</t>
@@ -277,45 +273,13 @@
   </si>
   <si>
     <t>/sample_pages/page6/8.html</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user1</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user2</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user3</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user4</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user5</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user6</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user7</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>user8</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -326,37 +290,51 @@
       <sz val="8"/>
       <color rgb="FF333333"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="6"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="11"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="6">
@@ -492,6 +470,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -781,17 +767,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U24" sqref="U24"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.625" defaultRowHeight="19" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="5" width="3" customWidth="1"/>
@@ -806,7 +792,7 @@
     <col min="18" max="18" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="10" customHeight="1">
+    <row r="1" spans="1:20" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,19 +815,18 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row r="3" spans="1:21" ht="37">
+    </row>
+    <row r="3" spans="1:20" ht="38.25" x14ac:dyDescent="0.85">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -894,71 +879,65 @@
       <c r="T7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="O8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="P8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="Q8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="R8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="S8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="T8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -969,14 +948,14 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4">
         <v>1</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="9"/>
@@ -984,15 +963,12 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
-      <c r="U9" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1002,7 +978,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4">
@@ -1011,25 +987,22 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R10" s="4">
         <v>1</v>
       </c>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
-      <c r="U10" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1039,7 +1012,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4">
@@ -1048,25 +1021,22 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R11" s="4">
         <v>1</v>
       </c>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
-      <c r="U11" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1076,7 +1046,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4">
@@ -1085,25 +1055,22 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R12" s="4">
         <v>1</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
-      <c r="U12" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1113,7 +1080,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4">
@@ -1122,25 +1089,22 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R13" s="4">
         <v>1</v>
       </c>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
-      <c r="U13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1150,7 +1114,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4">
@@ -1159,25 +1123,22 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R14" s="4">
         <v>1</v>
       </c>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1187,7 +1148,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4">
@@ -1196,26 +1157,23 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R15" s="4">
         <v>1</v>
       </c>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1224,7 +1182,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4">
@@ -1233,26 +1191,23 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R16" s="4">
         <v>1</v>
       </c>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1261,7 +1216,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4">
@@ -1270,26 +1225,23 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R17" s="4">
         <v>1</v>
       </c>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
-      <c r="U17" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1298,7 +1250,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4">
@@ -1307,26 +1259,23 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R18" s="4">
         <v>1</v>
       </c>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
-      <c r="U18" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1335,7 +1284,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4">
@@ -1344,26 +1293,23 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R19" s="4">
         <v>1</v>
       </c>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-      <c r="U19" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1372,7 +1318,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4">
@@ -1381,26 +1327,23 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R20" s="4">
         <v>1</v>
       </c>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
-      <c r="U20" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1409,7 +1352,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4">
@@ -1418,26 +1361,23 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R21" s="4">
         <v>1</v>
       </c>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
-      <c r="U21" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1446,7 +1386,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4">
@@ -1455,26 +1395,23 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R22" s="4">
         <v>1</v>
       </c>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
-      <c r="U22" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1483,7 +1420,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4">
@@ -1492,25 +1429,22 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R23" s="4">
         <v>1</v>
       </c>
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
-      <c r="U23" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1520,7 +1454,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4">
@@ -1529,25 +1463,22 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R24" s="4">
         <v>1</v>
       </c>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
-      <c r="U24" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1557,7 +1488,7 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4">
@@ -1566,25 +1497,22 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R25" s="4">
         <v>1</v>
       </c>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
-      <c r="U25" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1594,7 +1522,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4">
@@ -1603,25 +1531,22 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R26" s="4">
         <v>1</v>
       </c>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
-      <c r="U26" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1631,10 +1556,10 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M27" s="4">
         <v>1</v>
@@ -1642,25 +1567,22 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R27" s="4">
         <v>1</v>
       </c>
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
-      <c r="U27" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1670,7 +1592,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4">
@@ -1679,23 +1601,20 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R28" s="4">
         <v>1</v>
       </c>
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
-      <c r="U28" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="5" customHeight="1">
+    </row>
+    <row r="31" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1716,7 +1635,6 @@
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>